<commit_message>
Output Plots for nodes and system
</commit_message>
<xml_diff>
--- a/Thesis/fuel_states.xlsx
+++ b/Thesis/fuel_states.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rockmtnins-my.sharepoint.com/personal/abigail_weeks_rmi_org/Documents/Documents/GitHub/Thesis/Thesis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="56" documentId="8_{65F57FD0-643B-4C4B-AF6C-2E78FE78B136}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BB67B8EB-24B9-4555-90CE-FF853B8B575F}"/>
+  <xr:revisionPtr revIDLastSave="66" documentId="8_{65F57FD0-643B-4C4B-AF6C-2E78FE78B136}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A87857CF-E1F7-4540-8221-00BD7D23999F}"/>
   <bookViews>
-    <workbookView xWindow="-28905" yWindow="0" windowWidth="14610" windowHeight="15585" xr2:uid="{0F65274D-4779-4E1C-BF1E-1388AE3914D1}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{0F65274D-4779-4E1C-BF1E-1388AE3914D1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,14 +36,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>fuel_type</t>
   </si>
   <si>
-    <t>base_bid_price</t>
-  </si>
-  <si>
     <t>solar</t>
   </si>
   <si>
@@ -80,10 +77,16 @@
     <t>wind_offshore</t>
   </si>
   <si>
-    <t>hybrid</t>
-  </si>
-  <si>
-    <t>none</t>
+    <t>bid_price</t>
+  </si>
+  <si>
+    <t>atb_capex</t>
+  </si>
+  <si>
+    <t>atb_capex_multiplier</t>
+  </si>
+  <si>
+    <t>gas</t>
   </si>
 </sst>
 </file>
@@ -459,281 +462,320 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C63B81AE-84CE-411B-9949-4A4526E4E5FE}">
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.85546875" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" customWidth="1"/>
-    <col min="4" max="4" width="31.140625" customWidth="1"/>
-    <col min="5" max="5" width="37.140625" customWidth="1"/>
-    <col min="8" max="8" width="13.5703125" customWidth="1"/>
-    <col min="9" max="9" width="11.7109375" customWidth="1"/>
-    <col min="10" max="10" width="20.140625" customWidth="1"/>
+    <col min="1" max="3" width="14.81640625" customWidth="1"/>
+    <col min="4" max="4" width="18.1796875" customWidth="1"/>
+    <col min="5" max="5" width="18.453125" customWidth="1"/>
+    <col min="6" max="6" width="31.1796875" customWidth="1"/>
+    <col min="7" max="7" width="37.1796875" customWidth="1"/>
+    <col min="10" max="10" width="13.54296875" customWidth="1"/>
+    <col min="11" max="11" width="11.7265625" customWidth="1"/>
+    <col min="12" max="12" width="20.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I1" t="s">
-        <v>12</v>
+      <c r="B2">
+        <v>1483</v>
+      </c>
+      <c r="C2">
+        <v>0.3</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>3000</v>
+      </c>
+      <c r="F2">
+        <v>1000</v>
+      </c>
+      <c r="G2">
+        <v>2000</v>
+      </c>
+      <c r="H2">
+        <v>0.08</v>
+      </c>
+      <c r="I2">
+        <v>49</v>
+      </c>
+      <c r="J2">
+        <v>17547</v>
+      </c>
+      <c r="K2">
+        <v>24011</v>
+      </c>
+      <c r="L2">
+        <f>((J2*1000)/K2)/0.38</f>
+        <v>1923.1317225219143</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>3000</v>
-      </c>
-      <c r="D2">
-        <v>1000</v>
-      </c>
-      <c r="E2">
+      <c r="B3">
+        <v>2478</v>
+      </c>
+      <c r="C3">
+        <v>0.3</v>
+      </c>
+      <c r="D3">
+        <v>1.5</v>
+      </c>
+      <c r="E3">
+        <v>6000</v>
+      </c>
+      <c r="F3">
+        <v>4000</v>
+      </c>
+      <c r="G3">
         <v>2000</v>
       </c>
-      <c r="F2">
-        <v>0.08</v>
-      </c>
-      <c r="G2">
-        <v>49</v>
-      </c>
-      <c r="H2">
-        <v>17547</v>
-      </c>
-      <c r="I2">
-        <v>24011</v>
-      </c>
-      <c r="J2">
-        <f>((H2*1000)/I2)/0.38</f>
-        <v>1923.1317225219143</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3">
-        <v>1.5</v>
-      </c>
-      <c r="C3">
-        <v>6000</v>
-      </c>
-      <c r="D3">
-        <v>4000</v>
-      </c>
-      <c r="E3">
-        <v>2000</v>
-      </c>
-      <c r="F3">
+      <c r="H3">
         <f>(0.58+0.08)/2</f>
         <v>0.32999999999999996</v>
       </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
       <c r="J3">
         <v>0</v>
       </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4">
+        <v>2911</v>
+      </c>
+      <c r="C4">
+        <v>0.3</v>
+      </c>
+      <c r="D4">
         <v>2</v>
       </c>
-      <c r="C4">
+      <c r="E4">
         <v>4000</v>
       </c>
-      <c r="D4">
+      <c r="F4">
         <v>4000</v>
       </c>
-      <c r="E4">
+      <c r="G4">
         <v>0</v>
       </c>
-      <c r="F4">
+      <c r="H4">
         <v>0.57999999999999996</v>
       </c>
-      <c r="H4">
+      <c r="J4">
         <v>51</v>
       </c>
-      <c r="I4">
+      <c r="K4">
         <v>730.6</v>
       </c>
-      <c r="J4">
-        <f>H4*1000/I4</f>
+      <c r="L4">
+        <f>J4*1000/K4</f>
         <v>69.805639200656998</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
+        <v>2000.5</v>
+      </c>
+      <c r="C5">
+        <v>0.3</v>
+      </c>
+      <c r="D5">
         <v>2.5</v>
       </c>
-      <c r="C5">
+      <c r="E5">
         <v>5000</v>
       </c>
-      <c r="D5">
+      <c r="F5">
         <v>2500</v>
       </c>
-      <c r="E5">
+      <c r="G5">
         <v>2500</v>
       </c>
-      <c r="F5">
+      <c r="H5">
         <v>0.41</v>
       </c>
-      <c r="G5">
+      <c r="I5">
         <v>59</v>
       </c>
-      <c r="H5">
+      <c r="J5">
         <v>31384</v>
       </c>
-      <c r="I5">
+      <c r="K5">
         <v>24084.9</v>
       </c>
-      <c r="J5">
-        <f>(H5*1000/I5)/0.13</f>
+      <c r="L5">
+        <f>(J5*1000/K5)/0.13</f>
         <v>10023.516170521139</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="B6">
+        <v>1556</v>
+      </c>
+      <c r="C6">
+        <v>0.3</v>
+      </c>
+      <c r="D6">
         <v>3</v>
       </c>
-      <c r="C6">
+      <c r="E6">
         <v>8000</v>
       </c>
-      <c r="D6">
-        <f>C6/7</f>
+      <c r="F6">
+        <f>E6/7</f>
         <v>1142.8571428571429</v>
       </c>
-      <c r="E6">
-        <f>C6-D6</f>
+      <c r="G6">
+        <f>E6-F6</f>
         <v>6857.1428571428569</v>
       </c>
-      <c r="F6">
+      <c r="H6">
         <v>0.74</v>
       </c>
-      <c r="G6">
+      <c r="I6">
         <v>39</v>
       </c>
-      <c r="H6">
+      <c r="J6">
         <v>376249.8</v>
       </c>
-      <c r="I6">
+      <c r="K6">
         <v>168654.1</v>
       </c>
-      <c r="J6">
-        <f>(H6*1000/I6)/0.71</f>
+      <c r="L6">
+        <f>(J6*1000/K6)/0.71</f>
         <v>3142.107400737058</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B7">
+        <v>6318.5</v>
+      </c>
+      <c r="C7">
+        <v>0.3</v>
+      </c>
+      <c r="D7">
         <v>3</v>
       </c>
-      <c r="C7">
+      <c r="E7">
         <v>8000</v>
       </c>
-      <c r="D7">
-        <f>C7/7</f>
+      <c r="F7">
+        <f>E7/7</f>
         <v>1142.8571428571429</v>
       </c>
-      <c r="E7">
-        <f>C7-D7</f>
+      <c r="G7">
+        <f>E7-F7</f>
         <v>6857.1428571428569</v>
       </c>
-      <c r="F7">
+      <c r="H7">
         <v>0.74</v>
       </c>
-      <c r="G7">
+      <c r="I7">
         <v>39</v>
       </c>
-      <c r="H7">
+      <c r="J7">
         <v>376249.8</v>
       </c>
-      <c r="I7">
+      <c r="K7">
         <v>168654.1</v>
       </c>
-      <c r="J7">
-        <f>(H7*1000/I7)/0.71</f>
+      <c r="L7">
+        <f>(J7*1000/K7)/0.71</f>
         <v>3142.107400737058</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="D8">
         <v>3</v>
       </c>
-      <c r="C8">
+      <c r="E8">
         <v>8000</v>
       </c>
-      <c r="D8">
-        <f>C8/7</f>
+      <c r="F8">
+        <f>E8/7</f>
         <v>1142.8571428571429</v>
       </c>
-      <c r="E8">
-        <f>C8-D8</f>
+      <c r="G8">
+        <f>E8-F8</f>
         <v>6857.1428571428569</v>
       </c>
-      <c r="F8">
+      <c r="H8">
         <v>0.74</v>
       </c>
-      <c r="G8">
+      <c r="I8">
         <v>39</v>
       </c>
-      <c r="H8">
+      <c r="J8">
         <v>376249.8</v>
       </c>
-      <c r="I8">
+      <c r="K8">
         <v>168654.1</v>
       </c>
-      <c r="J8">
-        <f>(H8*1000/I8)/0.71</f>
+      <c r="L8">
+        <f>(J8*1000/K8)/0.71</f>
         <v>3142.107400737058</v>
       </c>
     </row>

</xml_diff>